<commit_message>
chore: v0.3.3 release – focus wells import (UTC fix), template updates, dashboards and popover UX
</commit_message>
<xml_diff>
--- a/focus_template.xlsx
+++ b/focus_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12255"/>
+    <workbookView windowWidth="13545" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="模板" sheetId="1" r:id="rId1"/>
@@ -1239,8 +1239,8 @@
   <sheetPr/>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -1503,7 +1503,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="1">
-        <v>45905.25</v>
+        <v>45905.5833333333</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>

</xml_diff>